<commit_message>
Solved issues of creation sequence and date for the orders table, added sinks and correct order to sequence tables and added a machine column to the setup Times table
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -493,7 +493,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -557,7 +557,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -589,7 +589,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -605,7 +605,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -621,7 +621,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -717,7 +717,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -733,7 +733,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-02-05 08:00:00</t>
+          <t>2/5/2024 8:00:00 AM</t>
         </is>
       </c>
       <c r="C19" t="n">

</xml_diff>